<commit_message>
Korrekturen nach erster Rückgabe
- bessere Kurve
- Erläuterung der Kurve angepasst
</commit_message>
<xml_diff>
--- a/Diagramme.xlsx
+++ b/Diagramme.xlsx
@@ -382,11 +382,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="249898960"/>
-        <c:axId val="249892688"/>
+        <c:axId val="329650424"/>
+        <c:axId val="329650816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="249898960"/>
+        <c:axId val="329650424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,12 +443,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249892688"/>
+        <c:crossAx val="329650816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="249892688"/>
+        <c:axId val="329650816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249898960"/>
+        <c:crossAx val="329650424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -930,11 +930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="249894256"/>
-        <c:axId val="249889552"/>
+        <c:axId val="329648464"/>
+        <c:axId val="329655520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="249894256"/>
+        <c:axId val="329648464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -993,12 +993,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249889552"/>
+        <c:crossAx val="329655520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="249889552"/>
+        <c:axId val="329655520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1056,7 +1056,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249894256"/>
+        <c:crossAx val="329648464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,15 +1353,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:forward val="5"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.3791959766869466"/>
-                  <c:y val="-0.29494536723967557"/>
+                  <c:x val="-0.243215524987658"/>
+                  <c:y val="-0.16571295636178063"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1618,11 +1619,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="249895432"/>
-        <c:axId val="249890336"/>
+        <c:axId val="329650032"/>
+        <c:axId val="329659440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="249895432"/>
+        <c:axId val="329650032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,12 +1680,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249890336"/>
+        <c:crossAx val="329659440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="249890336"/>
+        <c:axId val="329659440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,7 +1742,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249895432"/>
+        <c:crossAx val="329650032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2007,11 +2008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335631856"/>
-        <c:axId val="335630288"/>
+        <c:axId val="329655912"/>
+        <c:axId val="329647680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335631856"/>
+        <c:axId val="329655912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2070,12 +2071,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335630288"/>
+        <c:crossAx val="329647680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335630288"/>
+        <c:axId val="329647680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2133,7 +2134,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335631856"/>
+        <c:crossAx val="329655912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2457,8 +2458,11 @@
             <c:v>s ref</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2476,87 +2480,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:forward val="5"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.66745812773403324"/>
-                  <c:y val="-0.26731771736080162"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t>y = 0,026e</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
-                      <a:t>0,0355x</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1200"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$C$137:$C$144</c:f>
@@ -2623,7 +2546,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2831,11 +2754,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="337243288"/>
-        <c:axId val="337248776"/>
+        <c:axId val="329651208"/>
+        <c:axId val="329647288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="337243288"/>
+        <c:axId val="329651208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2948,12 +2871,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337248776"/>
+        <c:crossAx val="329647288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="337248776"/>
+        <c:axId val="329647288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3066,7 +2989,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337243288"/>
+        <c:crossAx val="329651208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3090,10 +3013,6 @@
       </c:legendEntry>
       <c:legendEntry>
         <c:idx val="4"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="5"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout/>
@@ -6374,8 +6293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:J144"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135:F144"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7892,7 +7811,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fehler nach zweite Rückkgabe korrigiert
theo Werte für r_s und r_p nun berechnet
</commit_message>
<xml_diff>
--- a/Diagramme.xlsx
+++ b/Diagramme.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Experiment 1</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Experiment 3</t>
-  </si>
-  <si>
-    <t>Intesität</t>
   </si>
   <si>
     <t>Experiment 4</t>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>100% wer</t>
+  </si>
+  <si>
+    <t>Intensität</t>
   </si>
 </sst>
 </file>
@@ -155,6 +155,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -382,11 +383,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="329650424"/>
-        <c:axId val="329650816"/>
+        <c:axId val="235623480"/>
+        <c:axId val="235624264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="329650424"/>
+        <c:axId val="235623480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,12 +444,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329650816"/>
+        <c:crossAx val="235624264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="329650816"/>
+        <c:axId val="235624264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +506,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329650424"/>
+        <c:crossAx val="235623480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -569,6 +570,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -930,11 +932,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="329648464"/>
-        <c:axId val="329655520"/>
+        <c:axId val="233136064"/>
+        <c:axId val="338809584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="329648464"/>
+        <c:axId val="233136064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -993,12 +995,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329655520"/>
+        <c:crossAx val="338809584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="329655520"/>
+        <c:axId val="338809584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1056,7 +1058,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329648464"/>
+        <c:crossAx val="233136064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1619,11 +1621,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="329650032"/>
-        <c:axId val="329659440"/>
+        <c:axId val="338807232"/>
+        <c:axId val="338809192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="329650032"/>
+        <c:axId val="338807232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,12 +1682,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329659440"/>
+        <c:crossAx val="338809192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="329659440"/>
+        <c:axId val="338809192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,7 +1744,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329650032"/>
+        <c:crossAx val="338807232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1806,6 +1808,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2008,11 +2011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="329655912"/>
-        <c:axId val="329647680"/>
+        <c:axId val="338812720"/>
+        <c:axId val="338809976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="329655912"/>
+        <c:axId val="338812720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90"/>
@@ -2071,12 +2074,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329647680"/>
+        <c:crossAx val="338809976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="329647680"/>
+        <c:axId val="338809976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2134,7 +2137,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329655912"/>
+        <c:crossAx val="338812720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2455,104 +2458,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>s ref</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Tabelle1!$C$137:$C$144</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Tabelle1!$E$137:$E$144</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.56999999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>p ref</c:v>
+            <c:v>r_s</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2563,7 +2469,301 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="2"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$151:$C$191</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$I$151:$I$191</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>5.25255996607778E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3425445436613074E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4509286261655014E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5787876167185918E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7274071883139155E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8983042356823896E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0932518388570014E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3143087454339955E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5638539680728178E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8446271933309197E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1597758083523977E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5129094738150173E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.9081633050926151E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.3502708684252719E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8446483538003703E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.3974914488805517E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.10015886604787359</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10707938548978699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.11482916054405959</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12351418105991559</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13325562699772681</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.14419200546848349</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.15648155908481479</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.17030496629776265</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1858683513113713</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.20340661617953307</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.22318710034461375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.24551356270584399</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.27073046785443255</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29922754099276683</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.33144453500303861</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.36787612808086417</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.40907684151631712</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.45566583516287534</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.50833140388853282</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.56783496333086547</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.63501427953529066</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.71078566692763701</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.79614485525971246</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.89216621151246145</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99999999999999978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>r_p</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
@@ -2576,170 +2776,266 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
-            <c:forward val="5"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.49894583882191018"/>
-                  <c:y val="-0.31980928086800398"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t>y = 9E-08x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
-                      <a:t>4</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t> - 1E-05x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
-                      <a:t>3</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t> + 0,0006x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="30000"/>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                      <a:t> - 0,0106x + 0,1019</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1200"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$137:$C$144</c:f>
+              <c:f>Tabelle1!$C$151:$C$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="26">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="31">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$F$137:$F$144</c:f>
+              <c:f>Tabelle1!$J$151:$J$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.04</c:v>
+                  <c:v>4.8584387910798062E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.04</c:v>
+                  <c:v>4.7722107250880455E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.03</c:v>
+                  <c:v>4.6701135274474226E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>4.5520817332930522E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>4.4180651812099667E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0000000000000004E-4</c:v>
+                  <c:v>4.2680421795508086E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.04</c:v>
+                  <c:v>4.1020361285155973E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23</c:v>
+                  <c:v>3.9201364000269016E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7225244837689235E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5095066647851655E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2815548197165E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0393573229968766E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7838825641407942E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5164582224597803E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.2388702649082392E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9534866769857717E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6634122723952233E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3726826426869447E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0865075208474673E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.115767001146721E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5644538369240158E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.3202073149051431E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5217781276874235E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.4541716485218842E-4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.4839785034474555E-5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.1396832624507196E-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1032961042229156E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.3410010000632131E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.411033015055772E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.4155326038502557E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.8427737970411338E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.814906612588526E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.4893277547942625E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.12069806131148915</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.16821594123890557</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.23092175817767993</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.31340097761354085</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.42175564459753212</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.56418443297643128</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.7518250457962502</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99999999999999933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2754,11 +3050,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="329651208"/>
-        <c:axId val="329647288"/>
+        <c:axId val="338814288"/>
+        <c:axId val="338808016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="329651208"/>
+        <c:axId val="338814288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2871,12 +3167,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329647288"/>
+        <c:crossAx val="338808016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="329647288"/>
+        <c:axId val="338808016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,7 +3285,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329651208"/>
+        <c:crossAx val="338814288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3003,18 +3299,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="4"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -6291,10 +6575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:J144"/>
+  <dimension ref="A5:J191"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="M126" sqref="M126"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="J151" sqref="J151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6810,7 +7094,7 @@
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56">
         <v>2.0019999999999998</v>
@@ -7177,17 +7461,17 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D91">
         <v>2.0219999999999998</v>
@@ -7207,7 +7491,7 @@
         <v>4</v>
       </c>
       <c r="G94" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H94" t="s">
         <v>1</v>
@@ -7391,12 +7675,12 @@
     </row>
     <row r="111" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D114">
         <v>2.06</v>
@@ -7416,7 +7700,7 @@
         <v>4</v>
       </c>
       <c r="G117" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H117" t="s">
         <v>1</v>
@@ -7600,7 +7884,7 @@
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C131">
         <v>57.75</v>
@@ -7611,16 +7895,16 @@
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" t="s">
         <v>14</v>
       </c>
-      <c r="D135" t="s">
+      <c r="E135" t="s">
         <v>15</v>
       </c>
-      <c r="E135" t="s">
+      <c r="F135" t="s">
         <v>16</v>
-      </c>
-      <c r="F135" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
@@ -7797,6 +8081,889 @@
       <c r="J144">
         <f t="shared" si="8"/>
         <v>0.23092992894820649</v>
+      </c>
+    </row>
+    <row r="149" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" t="s">
+        <v>14</v>
+      </c>
+      <c r="E149" t="s">
+        <v>15</v>
+      </c>
+      <c r="F149" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I150" t="s">
+        <v>15</v>
+      </c>
+      <c r="J150" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="151" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <v>10</v>
+      </c>
+      <c r="D151">
+        <f>DEGREES(ASIN(G151))</f>
+        <v>6.309776428730574</v>
+      </c>
+      <c r="G151">
+        <f>(1/1.58)*SIN(RADIANS(C151))</f>
+        <v>0.10990390991577868</v>
+      </c>
+      <c r="I151">
+        <f>(SIN(RADIANS(C151-D151))/(SIN(RADIANS(C151+D151))))^2</f>
+        <v>5.25255996607778E-2</v>
+      </c>
+      <c r="J151">
+        <f>(TAN(RADIANS(C151-D151))/(TAN(RADIANS(C151+D151))))^2</f>
+        <v>4.8584387910798062E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <v>12</v>
+      </c>
+      <c r="D152">
+        <f t="shared" ref="D152:D191" si="9">DEGREES(ASIN(G152))</f>
+        <v>7.561463373886828</v>
+      </c>
+      <c r="G152">
+        <f t="shared" ref="G152:G191" si="10">(1/1.58)*SIN(RADIANS(C152))</f>
+        <v>0.13158967773275906</v>
+      </c>
+      <c r="I152">
+        <f t="shared" ref="I152:I191" si="11">(SIN(RADIANS(C152-D152))/(SIN(RADIANS(C152+D152))))^2</f>
+        <v>5.3425445436613074E-2</v>
+      </c>
+      <c r="J152">
+        <f t="shared" ref="J152:J191" si="12">(TAN(RADIANS(C152-D152))/(TAN(RADIANS(C152+D152))))^2</f>
+        <v>4.7722107250880455E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <v>14</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="9"/>
+        <v>8.8074959432728122</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="10"/>
+        <v>0.15311512379725803</v>
+      </c>
+      <c r="I153">
+        <f t="shared" si="11"/>
+        <v>5.4509286261655014E-2</v>
+      </c>
+      <c r="J153">
+        <f t="shared" si="12"/>
+        <v>4.6701135274474226E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <v>16</v>
+      </c>
+      <c r="D154">
+        <f t="shared" si="9"/>
+        <v>10.046887175658268</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="10"/>
+        <v>0.1744540226689868</v>
+      </c>
+      <c r="I154">
+        <f t="shared" si="11"/>
+        <v>5.5787876167185918E-2</v>
+      </c>
+      <c r="J154">
+        <f t="shared" si="12"/>
+        <v>4.5520817332930522E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <v>18</v>
+      </c>
+      <c r="D155">
+        <f t="shared" si="9"/>
+        <v>11.278629540916732</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="10"/>
+        <v>0.19558037618667554</v>
+      </c>
+      <c r="I155">
+        <f t="shared" si="11"/>
+        <v>5.7274071883139155E-2</v>
+      </c>
+      <c r="J155">
+        <f t="shared" si="12"/>
+        <v>4.4180651812099667E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C156">
+        <v>20</v>
+      </c>
+      <c r="D156">
+        <f t="shared" si="9"/>
+        <v>12.501692019371907</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="10"/>
+        <v>0.21646844514282829</v>
+      </c>
+      <c r="I156">
+        <f t="shared" si="11"/>
+        <v>5.8983042356823896E-2</v>
+      </c>
+      <c r="J156">
+        <f t="shared" si="12"/>
+        <v>4.2680421795508086E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C157">
+        <v>22</v>
+      </c>
+      <c r="D157">
+        <f t="shared" si="9"/>
+        <v>13.715017205580041</v>
+      </c>
+      <c r="G157">
+        <f t="shared" si="10"/>
+        <v>0.23709278064298225</v>
+      </c>
+      <c r="I157">
+        <f t="shared" si="11"/>
+        <v>6.0932518388570014E-2</v>
+      </c>
+      <c r="J157">
+        <f t="shared" si="12"/>
+        <v>4.1020361285155973E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <v>24</v>
+      </c>
+      <c r="D158">
+        <f t="shared" si="9"/>
+        <v>14.917518451036296</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="10"/>
+        <v>0.25742825511126594</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="11"/>
+        <v>6.3143087454339955E-2</v>
+      </c>
+      <c r="J158">
+        <f t="shared" si="12"/>
+        <v>3.9201364000269016E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <v>26</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="9"/>
+        <v>16.108077064798447</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="10"/>
+        <v>0.27745009290447936</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="11"/>
+        <v>6.5638539680728178E-2</v>
+      </c>
+      <c r="J159">
+        <f t="shared" si="12"/>
+        <v>3.7225244837689235E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C160">
+        <v>28</v>
+      </c>
+      <c r="D160">
+        <f t="shared" si="9"/>
+        <v>17.285539596259891</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="10"/>
+        <v>0.29713390049739924</v>
+      </c>
+      <c r="I160">
+        <f t="shared" si="11"/>
+        <v>6.8446271933309197E-2</v>
+      </c>
+      <c r="J160">
+        <f t="shared" si="12"/>
+        <v>3.5095066647851655E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C161">
+        <v>30</v>
+      </c>
+      <c r="D161">
+        <f t="shared" si="9"/>
+        <v>18.448715230321213</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="10"/>
+        <v>0.31645569620253156</v>
+      </c>
+      <c r="I161">
+        <f t="shared" si="11"/>
+        <v>7.1597758083523977E-2</v>
+      </c>
+      <c r="J161">
+        <f t="shared" si="12"/>
+        <v>3.2815548197165E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C162">
+        <v>32</v>
+      </c>
+      <c r="D162">
+        <f t="shared" si="9"/>
+        <v>19.596373332038933</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="10"/>
+        <v>0.33539193938810435</v>
+      </c>
+      <c r="I162">
+        <f t="shared" si="11"/>
+        <v>7.5129094738150173E-2</v>
+      </c>
+      <c r="J162">
+        <f t="shared" si="12"/>
+        <v>3.0393573229968766E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C163">
+        <v>34</v>
+      </c>
+      <c r="D163">
+        <f t="shared" si="9"/>
+        <v>20.72724118548048</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="10"/>
+        <v>0.35391955915870055</v>
+      </c>
+      <c r="I163">
+        <f t="shared" si="11"/>
+        <v>7.9081633050926151E-2</v>
+      </c>
+      <c r="J163">
+        <f t="shared" si="12"/>
+        <v>2.7838825641407942E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C164">
+        <v>36</v>
+      </c>
+      <c r="D164">
+        <f t="shared" si="9"/>
+        <v>21.840001979963578</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="10"/>
+        <v>0.37201598246359058</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="11"/>
+        <v>8.3502708684252719E-2</v>
+      </c>
+      <c r="J164">
+        <f t="shared" si="12"/>
+        <v>2.5164582224597803E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C165">
+        <v>38</v>
+      </c>
+      <c r="D165">
+        <f t="shared" si="9"/>
+        <v>22.933293106034668</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="10"/>
+        <v>0.38965916159851788</v>
+      </c>
+      <c r="I165">
+        <f t="shared" si="11"/>
+        <v>8.8446483538003703E-2</v>
+      </c>
+      <c r="J165">
+        <f t="shared" si="12"/>
+        <v>2.2388702649082392E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C166">
+        <v>40</v>
+      </c>
+      <c r="D166">
+        <f t="shared" si="9"/>
+        <v>24.005704833312411</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="10"/>
+        <v>0.40682760106742988</v>
+      </c>
+      <c r="I166">
+        <f t="shared" si="11"/>
+        <v>9.3974914488805517E-2</v>
+      </c>
+      <c r="J166">
+        <f t="shared" si="12"/>
+        <v>1.9534866769857717E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C167">
+        <v>42</v>
+      </c>
+      <c r="D167">
+        <f t="shared" si="9"/>
+        <v>25.055779452474756</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="10"/>
+        <v>0.42350038377142923</v>
+      </c>
+      <c r="I167">
+        <f t="shared" si="11"/>
+        <v>0.10015886604787359</v>
+      </c>
+      <c r="J167">
+        <f t="shared" si="12"/>
+        <v>1.6634122723952233E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C168">
+        <v>44</v>
+      </c>
+      <c r="D168">
+        <f t="shared" si="9"/>
+        <v>26.082010973886451</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="10"/>
+        <v>0.4396571964930362</v>
+      </c>
+      <c r="I168">
+        <f t="shared" si="11"/>
+        <v>0.10707938548978699</v>
+      </c>
+      <c r="J168">
+        <f t="shared" si="12"/>
+        <v>1.3726826426869447E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C169">
+        <v>46</v>
+      </c>
+      <c r="D169">
+        <f t="shared" si="9"/>
+        <v>27.082845485212761</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="10"/>
+        <v>0.45527835464471583</v>
+      </c>
+      <c r="I169">
+        <f t="shared" si="11"/>
+        <v>0.11482916054405959</v>
+      </c>
+      <c r="J169">
+        <f t="shared" si="12"/>
+        <v>1.0865075208474673E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C170">
+        <v>48</v>
+      </c>
+      <c r="D170">
+        <f t="shared" si="9"/>
+        <v>28.056682279266845</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="10"/>
+        <v>0.4703448262515153</v>
+      </c>
+      <c r="I170">
+        <f t="shared" si="11"/>
+        <v>0.12351418105991559</v>
+      </c>
+      <c r="J170">
+        <f t="shared" si="12"/>
+        <v>8.115767001146721E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C171">
+        <v>50</v>
+      </c>
+      <c r="D171">
+        <f t="shared" si="9"/>
+        <v>29.001875870561346</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="10"/>
+        <v>0.48483825513859363</v>
+      </c>
+      <c r="I171">
+        <f t="shared" si="11"/>
+        <v>0.13325562699772681</v>
+      </c>
+      <c r="J171">
+        <f t="shared" si="12"/>
+        <v>5.5644538369240158E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C172">
+        <v>52</v>
+      </c>
+      <c r="D172">
+        <f t="shared" si="9"/>
+        <v>29.916739023681867</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="10"/>
+        <v>0.49874098329539363</v>
+      </c>
+      <c r="I172">
+        <f t="shared" si="11"/>
+        <v>0.14419200546848349</v>
+      </c>
+      <c r="J172">
+        <f t="shared" si="12"/>
+        <v>3.3202073149051431E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C173">
+        <v>54</v>
+      </c>
+      <c r="D173">
+        <f t="shared" si="9"/>
+        <v>30.799546917616645</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="10"/>
+        <v>0.51203607238920723</v>
+      </c>
+      <c r="I173">
+        <f t="shared" si="11"/>
+        <v>0.15648155908481479</v>
+      </c>
+      <c r="J173">
+        <f t="shared" si="12"/>
+        <v>1.5217781276874235E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C174">
+        <v>56</v>
+      </c>
+      <c r="D174">
+        <f t="shared" si="9"/>
+        <v>31.648542566374193</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="10"/>
+        <v>0.52470732440192513</v>
+      </c>
+      <c r="I174">
+        <f t="shared" si="11"/>
+        <v>0.17030496629776265</v>
+      </c>
+      <c r="J174">
+        <f t="shared" si="12"/>
+        <v>3.4541716485218842E-4</v>
+      </c>
+    </row>
+    <row r="175" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C175">
+        <v>58</v>
+      </c>
+      <c r="D175">
+        <f t="shared" si="9"/>
+        <v>32.461943606319892</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="10"/>
+        <v>0.5367393013648265</v>
+      </c>
+      <c r="I175">
+        <f t="shared" si="11"/>
+        <v>0.1858683513113713</v>
+      </c>
+      <c r="J175">
+        <f t="shared" si="12"/>
+        <v>1.4839785034474555E-5</v>
+      </c>
+    </row>
+    <row r="176" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C176">
+        <v>60</v>
+      </c>
+      <c r="D176">
+        <f t="shared" si="9"/>
+        <v>33.237950543379959</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="10"/>
+        <v>0.54811734416736613</v>
+      </c>
+      <c r="I176">
+        <f t="shared" si="11"/>
+        <v>0.20340661617953307</v>
+      </c>
+      <c r="J176">
+        <f t="shared" si="12"/>
+        <v>8.1396832624507196E-4</v>
+      </c>
+    </row>
+    <row r="177" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C177">
+        <v>62</v>
+      </c>
+      <c r="D177">
+        <f t="shared" si="9"/>
+        <v>33.974756527413291</v>
+      </c>
+      <c r="G177">
+        <f t="shared" si="10"/>
+        <v>0.55882759041704222</v>
+      </c>
+      <c r="I177">
+        <f t="shared" si="11"/>
+        <v>0.22318710034461375</v>
+      </c>
+      <c r="J177">
+        <f t="shared" si="12"/>
+        <v>3.1032961042229156E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C178">
+        <v>64</v>
+      </c>
+      <c r="D178">
+        <f t="shared" si="9"/>
+        <v>34.670558685712493</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="10"/>
+        <v>0.56885699132858669</v>
+      </c>
+      <c r="I178">
+        <f t="shared" si="11"/>
+        <v>0.24551356270584399</v>
+      </c>
+      <c r="J178">
+        <f t="shared" si="12"/>
+        <v>7.3410010000632131E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C179">
+        <v>66</v>
+      </c>
+      <c r="D179">
+        <f t="shared" si="9"/>
+        <v>35.323571002270448</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="10"/>
+        <v>0.57819332762189923</v>
+      </c>
+      <c r="I179">
+        <f t="shared" si="11"/>
+        <v>0.27073046785443255</v>
+      </c>
+      <c r="J179">
+        <f t="shared" si="12"/>
+        <v>1.411033015055772E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C180">
+        <v>68</v>
+      </c>
+      <c r="D180">
+        <f t="shared" si="9"/>
+        <v>35.932038674281458</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="10"/>
+        <v>0.58682522440935903</v>
+      </c>
+      <c r="I180">
+        <f t="shared" si="11"/>
+        <v>0.29922754099276683</v>
+      </c>
+      <c r="J180">
+        <f t="shared" si="12"/>
+        <v>2.4155326038502557E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C181">
+        <v>70</v>
+      </c>
+      <c r="D181">
+        <f t="shared" si="9"/>
+        <v>36.494253813316746</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="10"/>
+        <v>0.59474216505437227</v>
+      </c>
+      <c r="I181">
+        <f t="shared" si="11"/>
+        <v>0.33144453500303861</v>
+      </c>
+      <c r="J181">
+        <f t="shared" si="12"/>
+        <v>3.8427737970411338E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C182">
+        <v>72</v>
+      </c>
+      <c r="D182">
+        <f t="shared" si="9"/>
+        <v>37.008572287713889</v>
+      </c>
+      <c r="G182">
+        <f t="shared" si="10"/>
+        <v>0.60193450398427428</v>
+      </c>
+      <c r="I182">
+        <f t="shared" si="11"/>
+        <v>0.36787612808086417</v>
+      </c>
+      <c r="J182">
+        <f t="shared" si="12"/>
+        <v>5.814906612588526E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C183">
+        <v>74</v>
+      </c>
+      <c r="D183">
+        <f t="shared" si="9"/>
+        <v>37.47343142805105</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="10"/>
+        <v>0.60839347844197389</v>
+      </c>
+      <c r="I183">
+        <f t="shared" si="11"/>
+        <v>0.40907684151631712</v>
+      </c>
+      <c r="J183">
+        <f t="shared" si="12"/>
+        <v>8.4893277547942625E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C184">
+        <v>76</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="9"/>
+        <v>37.887368243357749</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="10"/>
+        <v>0.61411121916202305</v>
+      </c>
+      <c r="I184">
+        <f t="shared" si="11"/>
+        <v>0.45566583516287534</v>
+      </c>
+      <c r="J184">
+        <f t="shared" si="12"/>
+        <v>0.12069806131148915</v>
+      </c>
+    </row>
+    <row r="185" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C185">
+        <v>78</v>
+      </c>
+      <c r="D185">
+        <f t="shared" si="9"/>
+        <v>38.249037727118484</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="10"/>
+        <v>0.61908075995810474</v>
+      </c>
+      <c r="I185">
+        <f t="shared" si="11"/>
+        <v>0.50833140388853282</v>
+      </c>
+      <c r="J185">
+        <f t="shared" si="12"/>
+        <v>0.16821594123890557</v>
+      </c>
+    </row>
+    <row r="186" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C186">
+        <v>80</v>
+      </c>
+      <c r="D186">
+        <f t="shared" si="9"/>
+        <v>38.557230774973377</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="10"/>
+        <v>0.62329604621025814</v>
+      </c>
+      <c r="I186">
+        <f t="shared" si="11"/>
+        <v>0.56783496333086547</v>
+      </c>
+      <c r="J186">
+        <f t="shared" si="12"/>
+        <v>0.23092175817767993</v>
+      </c>
+    </row>
+    <row r="187" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C187">
+        <v>82</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="9"/>
+        <v>38.810891196277936</v>
+      </c>
+      <c r="G187">
+        <f t="shared" si="10"/>
+        <v>0.62675194224150022</v>
+      </c>
+      <c r="I187">
+        <f t="shared" si="11"/>
+        <v>0.63501427953529066</v>
+      </c>
+      <c r="J187">
+        <f t="shared" si="12"/>
+        <v>0.31340097761354085</v>
+      </c>
+    </row>
+    <row r="188" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C188">
+        <v>84</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="9"/>
+        <v>39.009131284836975</v>
+      </c>
+      <c r="G188">
+        <f t="shared" si="10"/>
+        <v>0.62944423757485646</v>
+      </c>
+      <c r="I188">
+        <f t="shared" si="11"/>
+        <v>0.71078566692763701</v>
+      </c>
+      <c r="J188">
+        <f t="shared" si="12"/>
+        <v>0.42175564459753212</v>
+      </c>
+    </row>
+    <row r="189" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C189">
+        <v>86</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="9"/>
+        <v>39.151245424468364</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="10"/>
+        <v>0.63136965206317985</v>
+      </c>
+      <c r="I189">
+        <f t="shared" si="11"/>
+        <v>0.79614485525971246</v>
+      </c>
+      <c r="J189">
+        <f t="shared" si="12"/>
+        <v>0.56418443297643128</v>
+      </c>
+    </row>
+    <row r="190" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C190">
+        <v>88</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="9"/>
+        <v>39.236721245001597</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="10"/>
+        <v>0.63252583988550359</v>
+      </c>
+      <c r="I190">
+        <f t="shared" si="11"/>
+        <v>0.89216621151246145</v>
+      </c>
+      <c r="J190">
+        <f t="shared" si="12"/>
+        <v>0.7518250457962502</v>
+      </c>
+    </row>
+    <row r="191" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C191">
+        <v>90</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="9"/>
+        <v>39.265247913879456</v>
+      </c>
+      <c r="G191">
+        <f t="shared" si="10"/>
+        <v>0.63291139240506322</v>
+      </c>
+      <c r="I191">
+        <f t="shared" si="11"/>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="J191">
+        <f t="shared" si="12"/>
+        <v>0.99999999999999933</v>
       </c>
     </row>
   </sheetData>
@@ -7811,7 +8978,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>